<commit_message>
Add AI Rubric Canvas entry to list.xlsx
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -481,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2149,7 +2149,32 @@
       </c>
     </row>
     <row r="77">
-      <c r="E77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>AI-Assisted Rubric Creation for Canvas LMS</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>ai-rubric-canvas.html</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="E78">
         <f>SUM(E2:E76)</f>
         <v/>
       </c>

</xml_diff>